<commit_message>
Reduit poids img 9,51 à 3,56
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\PROJET4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\P4_MADJIASSOUM_ELYSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA376A5-A6B8-4BF6-BA8D-794587FC41E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B317F4-E531-43E9-9801-E43A62286F18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Catégorie</t>
   </si>
@@ -97,13 +97,16 @@
   <si>
     <t xml:space="preserve">bloc img col-sm-12
 </t>
+  </si>
+  <si>
+    <t>https://validator.w3.org/checklink?uri=https%3A%2F%2Fmadjiassoum.github.io%2FP4_MADJIASSOUM_ELYSEE%2Favant%2F&amp;hide_type=all&amp;depth=&amp;check=Check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +151,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,10 +204,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,8 +234,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -451,7 +465,7 @@
     <col min="3" max="3" width="26.77734375" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -605,7 +619,9 @@
       <c r="E9" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="5"/>
@@ -1653,7 +1669,10 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{31302C84-9100-4748-926C-2B8197DF42DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reduit poids img de 9,51 à 3,56
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\P4_MADJIASSOUM_ELYSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B317F4-E531-43E9-9801-E43A62286F18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012015F-C4FE-4B9F-9736-0FABC46B8493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Catégorie</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>https://validator.w3.org/checklink?uri=https%3A%2F%2Fmadjiassoum.github.io%2FP4_MADJIASSOUM_ELYSEE%2Favant%2F&amp;hide_type=all&amp;depth=&amp;check=Check</t>
+  </si>
+  <si>
+    <t>Favicom</t>
+  </si>
+  <si>
+    <t>poids très élevé pouvant r</t>
+  </si>
+  <si>
+    <t>SEO</t>
   </si>
 </sst>
 </file>
@@ -455,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -634,9 +643,15 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Mod fichiers html pour semantique et correct erreur w3C
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\P4_MADJIASSOUM_ELYSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012015F-C4FE-4B9F-9736-0FABC46B8493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774F8180-0AF3-4DB6-886A-FBA3EBD5DE87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Catégorie</t>
   </si>
@@ -49,11 +49,6 @@
   </si>
   <si>
     <t>Accessibilité</t>
-  </si>
-  <si>
-    <t>Fichier index.html
-  Balise &lt;head&gt;
- Balise Title</t>
   </si>
   <si>
     <t>Il faut que le design soit inclusif, sans vrai title  celai ne va pas faciliter la tâche pour les personnes en situation d'handicap utilisant des lecteurs d'écran</t>
@@ -102,20 +97,68 @@
     <t>https://validator.w3.org/checklink?uri=https%3A%2F%2Fmadjiassoum.github.io%2FP4_MADJIASSOUM_ELYSEE%2Favant%2F&amp;hide_type=all&amp;depth=&amp;check=Check</t>
   </si>
   <si>
-    <t>Favicom</t>
-  </si>
-  <si>
-    <t>poids très élevé pouvant r</t>
-  </si>
-  <si>
     <t>SEO</t>
+  </si>
+  <si>
+    <t>Favicom poids &gt; à 10 KiloOctet</t>
+  </si>
+  <si>
+    <t>Il sera chargé automatiquementet devrait avoir un en-tête dans un futur lointain</t>
+  </si>
+  <si>
+    <t>Il faut reduire le poids du favicon &lt;= 2 kiloOctet</t>
+  </si>
+  <si>
+    <t>yslow.org/faq/</t>
+  </si>
+  <si>
+    <t>SPECIFIEZ LES TAILLES D'IMAGE</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/TR/mobile-bp/#ImageSize</t>
+  </si>
+  <si>
+    <t>Il manque soit le width soit la hauteur</t>
+  </si>
+  <si>
+    <t>Il faut que les dimensions de l'img ne depassent pas son container</t>
+  </si>
+  <si>
+    <t>CSS minification</t>
+  </si>
+  <si>
+    <t>Alignement des après les virgules au lieu de faire des retours à la ligne. Aussi à supprimer les espaces vide entre les blocs.</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/TR/mobile-bp/</t>
+  </si>
+  <si>
+    <t>Compression des espaces blancs</t>
+  </si>
+  <si>
+    <t>Texte en img</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ce texte n'est pas sélectionnable, </t>
+  </si>
+  <si>
+    <t>https://accessibility.belgium.be/fr/articles/images/utilisez-du-vrai-texte-et-pas-du-texte-sous-forme-dimage</t>
+  </si>
+  <si>
+    <t>14 img en png, jpg, bmp</t>
+  </si>
+  <si>
+    <t>Poids très élevés</t>
+  </si>
+  <si>
+    <t>Compression reduisant le poids de 9,51 Mégaoctet à 3,21 MégaOctet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,6 +210,27 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -217,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +308,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -462,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -531,94 +604,88 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="41.25" customHeight="1">
+    <row r="4" spans="1:26" s="10" customFormat="1" ht="107.25" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
+      <c r="B4" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="12" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="79.5" customHeight="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:26" s="10" customFormat="1" ht="107.25" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:26" ht="41.25" customHeight="1">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+    <row r="7" spans="1:26" ht="79.5" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="93" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="5"/>
       <c r="B8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
@@ -628,93 +695,151 @@
       <c r="E9" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+    <row r="10" spans="1:26" ht="93" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+    <row r="12" spans="1:26" ht="87" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E12" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+    <row r="13" spans="1:26" ht="68.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E13" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+    <row r="14" spans="1:26" ht="87.75" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="E14" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+    <row r="15" spans="1:26" ht="66" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="E15" s="6" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1683,11 +1808,17 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{31302C84-9100-4748-926C-2B8197DF42DF}"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{31302C84-9100-4748-926C-2B8197DF42DF}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{2A8EC792-A26F-4666-930F-C7A44C6BF167}"/>
+    <hyperlink ref="F12" r:id="rId3" location="ImageSize" xr:uid="{95850C49-56C4-49A3-9737-A29561FD0430}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{D7475675-B318-45F0-A0EC-5DF8982A6B07}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{6A375AFC-E2EB-4B2C-BA15-0621F4308CDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mis en page avant 1er vrai test d'opimisat
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\P4_MADJIASSOUM_ELYSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923DC69B-6F31-4BD4-A974-B08518E937D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1583609-D3B2-46A3-A757-69AFEC99E735}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Catégorie</t>
   </si>
@@ -187,12 +187,6 @@
   </si>
   <si>
     <t>div Bouton CONTACT du bloc 1</t>
-  </si>
-  <si>
-    <t>Il n'y a rien à envoyer en dessous du titre h1</t>
-  </si>
-  <si>
-    <t>J'ai supprimé le premier bouton, et amélioré le deuxieme se trouvant dans le bloc</t>
   </si>
   <si>
     <t>&amp;rsquo;  &amp;gt;</t>
@@ -304,6 +298,15 @@
   </si>
   <si>
     <t>https://jigsaw.w3.org/css-validator/validator#errors</t>
+  </si>
+  <si>
+    <t>http://www.bhinformatique.fr/</t>
+  </si>
+  <si>
+    <t>J'ai supprimé le premier bouton, et amélioré le deuxieme se trouvant dans le bloc. Assimilé à du BLACK HAT ces répétitions</t>
+  </si>
+  <si>
+    <t>Il n'y a rien à envoyer en dessous du titre H1</t>
   </si>
 </sst>
 </file>
@@ -918,7 +921,7 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -995,7 +998,7 @@
       <c r="E3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1074,19 +1077,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>58</v>
       </c>
       <c r="E8" s="19" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1228,7 +1231,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>48</v>
@@ -1243,40 +1246,44 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="19" t="b">
         <v>0</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1284,25 +1291,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>68</v>
       </c>
       <c r="E20" s="19" t="b">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="5"/>
@@ -1314,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="5"/>
@@ -1324,7 +1331,7 @@
     <row r="23" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="24"/>
       <c r="D23" s="5"/>
@@ -2356,8 +2363,10 @@
     <hyperlink ref="F8" r:id="rId8" xr:uid="{D4E1885E-527F-4D26-AE47-2054EC443EC6}"/>
     <hyperlink ref="F19" r:id="rId9" xr:uid="{B8058F59-7FBC-42B1-972E-3805EDCA1CF8}"/>
     <hyperlink ref="F20" r:id="rId10" location="errors" xr:uid="{461CD64D-9EF7-4AEE-8419-8EAC27B36277}"/>
+    <hyperlink ref="F18" r:id="rId11" xr:uid="{65E85BF2-AFBA-461C-9F1F-B0C46AF846B4}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{EAC5A444-1CC1-4C17-BFF1-6E3EE92CBF22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mes 10 recommandations en 1er
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\P4_MADJIASSOUM_ELYSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96269CC-6BA5-4F1C-9388-D1D2792ABBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A18DD4B-69F5-4E74-AD4E-7EC09CA3D4D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>Catégorie</t>
   </si>
@@ -55,14 +55,7 @@
 attribut Description</t>
   </si>
   <si>
-    <t>Balise méta
-attribut Keyword</t>
-  </si>
-  <si>
     <t>Manque du texte pour la description</t>
-  </si>
-  <si>
-    <t>répétition du terme  AGENCE DESIGN Black hat par Googlebot</t>
   </si>
   <si>
     <t>Image texte</t>
@@ -84,15 +77,6 @@
     <t>SEO</t>
   </si>
   <si>
-    <t>Favicom poids &gt; à 10 KiloOctet</t>
-  </si>
-  <si>
-    <t>Il sera chargé automatiquementet devrait avoir un en-tête dans un futur lointain</t>
-  </si>
-  <si>
-    <t>Il faut reduire le poids du favicon &lt;= 2 kiloOctet</t>
-  </si>
-  <si>
     <t>yslow.org/faq/</t>
   </si>
   <si>
@@ -102,12 +86,6 @@
     <t>http://www.w3.org/TR/mobile-bp/#ImageSize</t>
   </si>
   <si>
-    <t>Il manque soit le width soit la hauteur</t>
-  </si>
-  <si>
-    <t>Il faut que les dimensions de l'img ne depassent pas son container</t>
-  </si>
-  <si>
     <t>CSS minification</t>
   </si>
   <si>
@@ -132,18 +110,9 @@
     <t>14 img en png, jpg, bmp</t>
   </si>
   <si>
-    <t>Poids très élevés</t>
-  </si>
-  <si>
-    <t>Compression reduisant le poids de 9,51 Mégaoctet à 3,21 MégaOctet</t>
-  </si>
-  <si>
     <t>Une liste li vide dans nav</t>
   </si>
   <si>
-    <t>Il fait perdre de l'energie à Googlebot</t>
-  </si>
-  <si>
     <t>Suppresssion de cette liste li vide</t>
   </si>
   <si>
@@ -193,60 +162,6 @@
   </si>
   <si>
     <t>lang="Default"</t>
-  </si>
-  <si>
-    <t>Les navigateurs et autres applications peuvent utiliser des informations à propos de la langue du contenu pour offrir aux utilisateurs les informations les plus appropriées, ou pour présenter des informations aux utilisateurs de la manière la plus appropriée.</t>
-  </si>
-  <si>
-    <r>
-      <t>J'ai ajouté un attribut </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFA52A2A"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>lang</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> à la balise </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFA52A2A"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>html</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> pour définir la langue par défaut de la page.</t>
-    </r>
-  </si>
-  <si>
-    <t>    }</t>
-  </si>
-  <si>
-    <t>}</t>
   </si>
   <si>
     <t>Il ne permet pas le bon affichage de la page selon les ecrans</t>
@@ -259,32 +174,6 @@
  and (orientation: landscape)</t>
   </si>
   <si>
-    <t>Suppression  de ces parties  ajoutées</t>
-  </si>
-  <si>
-    <r>
-      <t>        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>padding-right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>: constant(safe-area-inset-right);</t>
-    </r>
-  </si>
-  <si>
     <t>constant(safe-area-inset-right); constant(safe-area-inset-left);</t>
   </si>
   <si>
@@ -306,14 +195,128 @@
     <t>Il n'y a rien à envoyer en dessous du titre H1</t>
   </si>
   <si>
-    <t>Suppression de cette répétition Assimilé au Black Hat par Google</t>
+    <t xml:space="preserve">22 Liens, Erreur 404 </t>
+  </si>
+  <si>
+    <t>Black hat. Ils ne sont pas importants, faisant perdre du temps</t>
+  </si>
+  <si>
+    <t>Les supprimer, differencier les liens. Pour ne pas être assimilés aux spams. En créant de bons liens pour le SEO</t>
+  </si>
+  <si>
+    <t>Les Technologies d'assistance ne peuvent pas deviner les texte en Image. Ni sa selection pour  changer de couleur</t>
+  </si>
+  <si>
+    <t>Il en faut pour ’informer les moteurs de recherche ainsi que les internautes du contenu de la page.</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/</t>
+  </si>
+  <si>
+    <t>https://josselinleydier.com/seo/poids-image/</t>
+  </si>
+  <si>
+    <t>Les navigateurs et autres applications peuvent utiliser des informations à propos de la langue du contenu pour offrir aux utilisateurs les informations les plus appropriées, ou pour présenter des informations aux utilisateurs de la manière la plus appropr</t>
+  </si>
+  <si>
+    <t>J'ai ajouté un attribut lang à la balise html pour définir la langue par défaut de la page.</t>
+  </si>
+  <si>
+    <t>Répétition du terme AGENCE DESIGN, Black hat par Googlebot</t>
+  </si>
+  <si>
+    <t>Pas pris en compte par google et donc supprimer cette balise meta</t>
+  </si>
+  <si>
+    <t>Favicom poids &gt;à 10 KiloOctet</t>
+  </si>
+  <si>
+    <t>Il sera chargé automatiquement et devrait avoir un en-tête dans un futur lointain</t>
+  </si>
+  <si>
+    <t>Il faut reduire le poids du favicom &lt;= 2 KiloOctet</t>
+  </si>
+  <si>
+    <t>Poids très élevés. 9,51MegaOctet</t>
+  </si>
+  <si>
+    <t>Compression reduisant à 3,21 MégaOctet</t>
+  </si>
+  <si>
+    <t>Suppression  de ces parties  ajoutées aux @media</t>
+  </si>
+  <si>
+    <t>Balise meta attribut keyword</t>
+  </si>
+  <si>
+    <t>Il fait perdre de l'energie à Googlebot et occupe de la place mis en page</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>La bonne pratique , replacer par du texte, qu'on peut changer de couleur, de police, de taille ….facilement</t>
+  </si>
+  <si>
+    <t>Texte, taille, couleur, background</t>
+  </si>
+  <si>
+    <t>Le texte n'est pas visible et soit fin pas pratique pour lire</t>
+  </si>
+  <si>
+    <t>Utilisation de bonness pratiques SEO utilisant arriere-plan et couleur texte et taille sans oublier la police</t>
+  </si>
+  <si>
+    <t>https://web-color.aliasdmc.fr/contraste-couleur-text-fond-wcag.php</t>
+  </si>
+  <si>
+    <t>Les script de la balise head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manque dela propriété DEFER pour retarder son lancement, car ils font perdre du temps aux navigateurs </t>
+  </si>
+  <si>
+    <t>Ajout de DEFER pour permettre à ces fichiers de se lancer en arrière-plan après que la page soit complètement ouverte</t>
+  </si>
+  <si>
+    <t>1 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>2 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>3 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>4 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>5 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>10 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>9 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>8 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>7 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>6 SUR 10 RECOMMANDE</t>
+  </si>
+  <si>
+    <t>https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -331,29 +334,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -408,39 +388,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFA52A2A"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFD4D4D4"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -452,8 +399,28 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,8 +433,14 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -552,30 +525,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -588,118 +537,93 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -918,17 +842,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1011"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
@@ -954,7 +878,6 @@
         <v>5</v>
       </c>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -974,398 +897,381 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="b">
+      <c r="E2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="10" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="5" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="5" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C5" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="5" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="5" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D11" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" s="10" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+    <row r="16" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="12" t="s">
-        <v>31</v>
+      <c r="B16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="10" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="17" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="142.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="C20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5"/>
+    <row r="21" spans="1:6" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:26" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5"/>
-    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2346,27 +2252,27 @@
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" xr:uid="{31302C84-9100-4748-926C-2B8197DF42DF}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{2A8EC792-A26F-4666-930F-C7A44C6BF167}"/>
-    <hyperlink ref="F12" r:id="rId3" location="ImageSize" xr:uid="{95850C49-56C4-49A3-9737-A29561FD0430}"/>
-    <hyperlink ref="F14" r:id="rId4" xr:uid="{D7475675-B318-45F0-A0EC-5DF8982A6B07}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{6A375AFC-E2EB-4B2C-BA15-0621F4308CDE}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{A5CFDCF7-2A12-4149-841D-512176167DF5}"/>
-    <hyperlink ref="F17" r:id="rId7" xr:uid="{1A3D6829-B069-4B8B-ACE9-1C81DC7EBB6E}"/>
-    <hyperlink ref="F8" r:id="rId8" xr:uid="{D4E1885E-527F-4D26-AE47-2054EC443EC6}"/>
-    <hyperlink ref="F19" r:id="rId9" xr:uid="{B8058F59-7FBC-42B1-972E-3805EDCA1CF8}"/>
-    <hyperlink ref="F20" r:id="rId10" location="errors" xr:uid="{461CD64D-9EF7-4AEE-8419-8EAC27B36277}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{65E85BF2-AFBA-461C-9F1F-B0C46AF846B4}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{EAC5A444-1CC1-4C17-BFF1-6E3EE92CBF22}"/>
+    <hyperlink ref="F17" r:id="rId1" xr:uid="{D7475675-B318-45F0-A0EC-5DF8982A6B07}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{6A375AFC-E2EB-4B2C-BA15-0621F4308CDE}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{A5CFDCF7-2A12-4149-841D-512176167DF5}"/>
+    <hyperlink ref="F19" r:id="rId4" xr:uid="{1A3D6829-B069-4B8B-ACE9-1C81DC7EBB6E}"/>
+    <hyperlink ref="F21" r:id="rId5" location="errors" xr:uid="{461CD64D-9EF7-4AEE-8419-8EAC27B36277}"/>
+    <hyperlink ref="F20" r:id="rId6" xr:uid="{65E85BF2-AFBA-461C-9F1F-B0C46AF846B4}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{EAC5A444-1CC1-4C17-BFF1-6E3EE92CBF22}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{F575A548-590E-4D87-B0A0-8AC48C86CCBA}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{8B0FFDF8-9ACD-4307-A64A-4346A7044924}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{95186DB6-84AE-4B0C-AABE-6727AD2DEC54}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{7A572469-3832-4CF3-8E23-9907CF61D84B}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{2DA0C652-A521-4FE8-8DBD-CE906940D7DA}"/>
+    <hyperlink ref="F11" r:id="rId13" location="ImageSize" xr:uid="{590FE81E-43A2-4BE7-990E-A8815F8987E7}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{EEBF2305-EDE6-4498-A85E-67CAF8E1D964}"/>
+    <hyperlink ref="F3" r:id="rId15" xr:uid="{F47F4876-A4B5-4531-BF69-FAE03CC005BA}"/>
+    <hyperlink ref="F13" r:id="rId16" xr:uid="{EDF86D28-D63B-419C-81D5-246B127CBE42}"/>
+    <hyperlink ref="F12" r:id="rId17" xr:uid="{FF85D5B3-C771-4A7D-8B9D-80D15813274A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId13"/>
+  <pageSetup orientation="landscape" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>